<commit_message>
server static IP set
</commit_message>
<xml_diff>
--- a/templates/New_Hires.xlsx
+++ b/templates/New_Hires.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,12 +530,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jason</t>
+          <t>Rachel</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Poage</t>
+          <t>Tipton</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -543,25 +543,25 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>605 Winston / Salem - Retail</t>
+          <t>316 Louisville - Retail</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Technician</t>
+          <t>Operation Manager</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lee Huffman</t>
+          <t>Shannon Drabant</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>13901015</v>
+        <v>13901022</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>nihilem@gmail.com</t>
+          <t>rntipton@charter.net</t>
         </is>
       </c>
       <c r="I2" t="b">
@@ -569,12 +569,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2021-12-20T00:00:00</t>
+          <t>2021-12-30T00:00:00</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2021-12-20T00:00:00</t>
+          <t>2021-12-30T00:00:00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -589,10 +589,81 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2021-12-20T16:42:25.107</t>
+          <t>2022-01-01T17:04:20.363</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
+        <is>
+          <t>0001-01-01T00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Dirk</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Tomlinson</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>301 Evansville - Retail</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Technician</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Dakota Floyd</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>13901023</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>dtomlinson145@gmail.com</t>
+        </is>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2022-01-04T00:00:00</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2022-01-02T00:00:00</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0001-01-01T00:00:00</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>POB Completed</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>2022-01-03T14:39:15.637</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>0001-01-01T00:00:00</t>
         </is>

</xml_diff>